<commit_message>
added data kaji ulang
</commit_message>
<xml_diff>
--- a/Industri/Industri.xlsx
+++ b/Industri/Industri.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\System Dynamics\Github\system_dynamics_reference\Industri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F10121-D83C-45B1-B78D-655B30C3FE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9CB069-B369-4A98-8769-2FFD4B20D77A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data industri" sheetId="1" r:id="rId1"/>
-    <sheet name="Nilai Tambah" sheetId="2" r:id="rId2"/>
-    <sheet name="PDB Industri Harga 2000" sheetId="4" r:id="rId3"/>
-    <sheet name="Pengeluaran untuk Naker" sheetId="3" r:id="rId4"/>
+    <sheet name="Pertanian" sheetId="6" r:id="rId2"/>
+    <sheet name="Nilai Tambah" sheetId="2" r:id="rId3"/>
+    <sheet name="PDB Industri Harga 2000" sheetId="4" r:id="rId4"/>
+    <sheet name="Pengeluaran untuk Naker" sheetId="3" r:id="rId5"/>
+    <sheet name="Jabar" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Tahun</t>
   </si>
@@ -176,18 +178,32 @@
   <si>
     <t>Nilai Output Industri Besar sedang Menurut Subsektor (Milyar rupiah) , 2000-2011</t>
   </si>
+  <si>
+    <t>Makanan dan Minuman (Milyar)</t>
+  </si>
+  <si>
+    <t>Luas Panen (ha)</t>
+  </si>
+  <si>
+    <t>Produktivitas (ku/ha)</t>
+  </si>
+  <si>
+    <t>Produksi (ton)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="####\ ###\ ###\ ##0.0"/>
-    <numFmt numFmtId="168" formatCode="###\ ##0"/>
-    <numFmt numFmtId="169" formatCode="#\ ###\ ##0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="####\ ###\ ###\ ##0.0"/>
+    <numFmt numFmtId="165" formatCode="###\ ##0"/>
+    <numFmt numFmtId="166" formatCode="#\ ###\ ##0"/>
+    <numFmt numFmtId="167" formatCode="###\ ###\ ##0"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,8 +564,31 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,8 +810,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002142"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1011,8 +1056,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1107,8 +1174,9 @@
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1123,25 +1191,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="39" fillId="34" borderId="15" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="39" fillId="34" borderId="15" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="39" fillId="39" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="39" fillId="39" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="39" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="36" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="41" fillId="36" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="35" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1150,17 +1209,17 @@
     <xf numFmtId="0" fontId="41" fillId="35" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="39" fillId="0" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="38" fillId="0" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="38" fillId="34" borderId="15" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="34" borderId="15" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="39" fillId="34" borderId="14" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="39" fillId="34" borderId="14" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1173,63 +1232,97 @@
     <xf numFmtId="0" fontId="41" fillId="34" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="41" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="41" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="39" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="39" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="39" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="34" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="39" fillId="38" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="37" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="36" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="34" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="36" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="18" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="37" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="39" fillId="38" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="39" fillId="37" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="39" fillId="36" borderId="10" xfId="92" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="39" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="37" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="36" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="94">
+  <cellStyles count="95">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="59" xr:uid="{93292353-1C63-4EFD-A090-F801C49903D5}"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
@@ -1290,6 +1383,7 @@
     <cellStyle name="Calculation 2" xfId="74" xr:uid="{13017354-0E71-4FE7-94DC-AA21D4581BDA}"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Check Cell 2" xfId="71" xr:uid="{ABC3C9C2-FCBC-447B-ACF0-8B100183C617}"/>
+    <cellStyle name="Comma" xfId="94" builtinId="3"/>
     <cellStyle name="Comma [0] 2" xfId="67" xr:uid="{1C820A21-3A44-4D9B-B2AF-E64B39A13D5E}"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Explanatory Text 2" xfId="63" xr:uid="{5CEE2697-E881-4456-8445-74F465DE3491}"/>
@@ -1614,6 +1708,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C97851A-2824-48BF-8D8C-C206FE756299}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="34">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="34">
+        <v>2018</v>
+      </c>
+      <c r="D2" s="34">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="34">
+        <v>2018</v>
+      </c>
+      <c r="F2" s="34">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
+        <v>11377934.439999999</v>
+      </c>
+      <c r="B3" s="35">
+        <v>10677887.15</v>
+      </c>
+      <c r="C3" s="35">
+        <v>52.03</v>
+      </c>
+      <c r="D3" s="35">
+        <v>51.14</v>
+      </c>
+      <c r="E3" s="36">
+        <v>59200533.719999999</v>
+      </c>
+      <c r="F3" s="36">
+        <v>54604033.340000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f>C3/10</f>
+        <v>5.2030000000000003</v>
+      </c>
+      <c r="D4" s="17">
+        <f>D3/10</f>
+        <v>5.1139999999999999</v>
+      </c>
+      <c r="E4" s="37">
+        <f>A3*C4</f>
+        <v>59199392.891319998</v>
+      </c>
+      <c r="F4" s="37">
+        <f>B3*D4</f>
+        <v>54606714.8851</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D60241-57A3-4230-AFBC-02450A5A3357}">
   <dimension ref="A2:Y24"/>
   <sheetViews>
@@ -1651,31 +1843,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2928,2003 +3120,2003 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB8CE4D-02FD-4279-8CC7-68132636FCCB}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="20"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="35"/>
-    </row>
-    <row r="2" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="20">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="42"/>
+    </row>
+    <row r="2" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="17">
         <v>2000</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="17">
         <v>2001</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="17">
         <v>2002</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="17">
         <v>2003</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="17">
         <v>2004</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="17">
         <v>2005</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="17">
         <v>2006</v>
       </c>
-      <c r="J2" s="20">
+      <c r="J2" s="17">
         <v>2007</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2" s="17">
         <v>2008</v>
       </c>
-      <c r="L2" s="20">
+      <c r="L2" s="17">
         <v>2009</v>
       </c>
-      <c r="M2" s="20">
+      <c r="M2" s="17">
         <v>2010</v>
       </c>
-      <c r="N2" s="20">
+      <c r="N2" s="17">
         <v>2011</v>
       </c>
-      <c r="O2" s="20">
+      <c r="O2" s="17">
         <v>2012</v>
       </c>
-      <c r="P2" s="20">
+      <c r="P2" s="17">
         <v>2013</v>
       </c>
-      <c r="Q2" s="20">
+      <c r="Q2" s="17">
         <v>2014</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <v>385597.9</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>398323.8</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>419387.8</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>441754.9</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="13">
         <v>469952.4</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="13">
         <v>491561.4</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="13">
         <v>514100.3</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="13">
         <v>538084.6</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="13">
         <v>557764.4</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="13">
         <v>570102.50000000012</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="13">
         <v>597134.89999999991</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="13">
         <v>633781.90000000014</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="13">
         <v>670190.60000000009</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="13">
         <v>707481.7</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="13">
         <v>741835.7</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <v>54279.8</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>50894.8</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>52179.5</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <v>52609.3</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="13">
         <v>51583.9</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="13">
         <v>48658.8</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="13">
         <v>47851.199999999997</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="13">
         <v>47823</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="13">
         <v>47662.7</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="13">
         <v>46934.899999999994</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="13">
         <v>47199.3</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="13">
         <v>46757.8</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="13">
         <v>45450.6</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="13">
         <v>44651.3</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="13">
         <v>43639.9</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>22602.9</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>22669.9</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>21820</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <v>22374.1</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <v>22322.3</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="12">
         <v>21207.200000000001</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="12">
         <v>20806.900000000001</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="12">
         <v>20780.599999999999</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="12">
         <v>20972</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="12">
         <v>21083.599999999999</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="12">
         <v>21346.5</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="12">
         <v>21459.7</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="12">
         <v>21046.5</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="12">
         <v>21286.5</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="12">
         <v>21566.5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>31676.9</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>28224.9</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>30359.5</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="12">
         <v>30235.200000000001</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="12">
         <v>29261.599999999999</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="12">
         <v>27451.599999999999</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="12">
         <v>27044.3</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="12">
         <v>27042.400000000001</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="12">
         <v>26690.699999999997</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="12">
         <v>25851.3</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="12">
         <v>25852.799999999999</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="12">
         <v>25298.1</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="12">
         <v>24404.1</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="12">
         <v>23364.800000000003</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="12">
         <v>22073.4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>331318.09999999998</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>347429</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>367208.3</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <v>389145.59999999998</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="13">
         <v>418368.5</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="13">
         <v>442902.6</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <v>466249.1</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <v>490261.6</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="13">
         <v>510101.70000000007</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="13">
         <v>523167.60000000009</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="13">
         <v>549935.59999999986</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="13">
         <v>587024.10000000009</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="13">
         <v>624740.00000000012</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="13">
         <v>662830.39999999991</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="13">
         <v>698195.79999999993</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="28">
         <v>112062.9</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>113256.6</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>113474.7</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <v>116528.6</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <v>118149.3</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="12">
         <v>121395.6</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="12">
         <v>130148.90000000001</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="12">
         <v>136722.40000000002</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="12">
         <v>139921.90000000002</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="12">
         <v>155620.20000000001</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="12">
         <v>159947.20000000001</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="12">
         <v>174566.7</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="12">
         <v>187787</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="12">
         <v>194063</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="12">
         <v>208105.4</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="27">
         <v>45421.599999999999</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>46966.2</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>48484.9</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <v>51483.6</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <v>53576.3</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="12">
         <v>54277.1</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="12">
         <v>54944.2</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="12">
         <v>52922.5</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="12">
         <v>50994</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="12">
         <v>51299.899999999994</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="12">
         <v>52206.2</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="12">
         <v>56131.1</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="12">
         <v>58527.100000000006</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="12">
         <v>62076.7</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="Q9" s="12">
         <v>63536.2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="26">
         <v>20275.400000000001</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>20384</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>20510.3</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <v>20754.3</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="12">
         <v>20325.5</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="12">
         <v>20138.5</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="12">
         <v>20006.2</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="12">
         <v>19657.599999999999</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="12">
         <v>20335.800000000003</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="12">
         <v>20055</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="12">
         <v>19359.7</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="12">
         <v>19427.399999999998</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="12">
         <v>18817.8</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="12">
         <v>19980.8</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="Q10" s="12">
         <v>21446.3</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>19997.900000000001</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>19043</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>20045.099999999999</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="12">
         <v>21731</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>23384.2</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="12">
         <v>23944.2</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="12">
         <v>24444.799999999996</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <v>25861</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="12">
         <v>25477.199999999997</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="12">
         <v>27092.400000000001</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="12">
         <v>27544.7</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="12">
         <v>27930.299999999996</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="12">
         <v>26603.5</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="12">
         <v>27786.1</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="12">
         <v>29494.6</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>42919.3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>43132.6</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>45171.4</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <v>50008.7</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="12">
         <v>54513.599999999999</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="12">
         <v>59293.1</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="12">
         <v>61947.899999999994</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="12">
         <v>65470</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="12">
         <v>68389.600000000006</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="12">
         <v>69514.2</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="12">
         <v>72782</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="12">
         <v>75657.5</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="12">
         <v>83598.200000000012</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="12">
         <v>85449.3</v>
       </c>
-      <c r="Q12" s="15">
+      <c r="Q12" s="12">
         <v>86530.8</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>10111.799999999999</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>12041.1</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>12830.6</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <v>13735.9</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <v>15045.2</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="12">
         <v>15618.1</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="12">
         <v>15700.099999999999</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="12">
         <v>16233.3</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="12">
         <v>15990.699999999999</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="12">
         <v>15908.9</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="12">
         <v>16255.599999999999</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="12">
         <v>17424.099999999999</v>
       </c>
-      <c r="O13" s="15">
+      <c r="O13" s="12">
         <v>18783.400000000001</v>
       </c>
-      <c r="P13" s="15">
+      <c r="P13" s="12">
         <v>19346.5</v>
       </c>
-      <c r="Q13" s="15">
+      <c r="Q13" s="12">
         <v>19640.300000000003</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>9142.6</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>9050.9</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>8935.5</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>8222.9</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <v>8008</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="12">
         <v>7712</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="12">
         <v>8076.8</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="12">
         <v>8213.2999999999993</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="12">
         <v>8044.7000000000007</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="12">
         <v>7702</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="12">
         <v>7885.6</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="12">
         <v>8915.2000000000007</v>
       </c>
-      <c r="O14" s="15">
+      <c r="O14" s="12">
         <v>9437.4000000000015</v>
       </c>
-      <c r="P14" s="15">
+      <c r="P14" s="12">
         <v>10091.1</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="Q14" s="12">
         <v>10515.8</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>68617.100000000006</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>80435.100000000006</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="12">
         <v>94982</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="12">
         <v>103414.7</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="12">
         <v>121683.3</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="12">
         <v>136744.6</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="12">
         <v>147063.79999999999</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="12">
         <v>161375.6</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="12">
         <v>177178.30000000002</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="12">
         <v>172085.1</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="12">
         <v>189947.89999999997</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="12">
         <v>202892</v>
       </c>
-      <c r="O15" s="15">
+      <c r="O15" s="12">
         <v>217152.1</v>
       </c>
-      <c r="P15" s="15">
+      <c r="P15" s="12">
         <v>240031.59999999998</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="Q15" s="12">
         <v>254564.09999999998</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>2769.5</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>3119.5</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="12">
         <v>2773.8</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="12">
         <v>3265.9</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>3683.1</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="12">
         <v>3779.4</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="12">
         <v>3916.3999999999996</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="12">
         <v>3805.8999999999996</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="12">
         <v>3769.5</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="12">
         <v>3889.8999999999996</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="12">
         <v>4006.7</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="12">
         <v>4079.7999999999997</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O16" s="12">
         <v>4033.5</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="12">
         <v>4005.3</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="Q16" s="12">
         <v>4362.3</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="15">
         <f>SUM(C8:C16,C5:C6)</f>
         <v>385597.9</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="15">
         <f t="shared" ref="D17:Q17" si="0">SUM(D8:D16,D5:D6)</f>
         <v>398323.80000000005</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="15">
         <f t="shared" si="0"/>
         <v>419387.8</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>441754.90000000008</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="15">
         <f t="shared" si="0"/>
         <v>469952.39999999997</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <f t="shared" si="0"/>
         <v>491561.39999999997</v>
       </c>
-      <c r="I17" s="18">
+      <c r="I17" s="15">
         <f t="shared" si="0"/>
         <v>514100.3</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="15">
         <f t="shared" si="0"/>
         <v>538084.6</v>
       </c>
-      <c r="K17" s="18">
+      <c r="K17" s="15">
         <f t="shared" si="0"/>
         <v>557764.4</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="15">
         <f t="shared" si="0"/>
         <v>570102.50000000012</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="15">
         <f t="shared" si="0"/>
         <v>597134.89999999991</v>
       </c>
-      <c r="N17" s="18">
+      <c r="N17" s="15">
         <f t="shared" si="0"/>
         <v>633781.9</v>
       </c>
-      <c r="O17" s="18">
+      <c r="O17" s="15">
         <f t="shared" si="0"/>
         <v>670190.60000000009</v>
       </c>
-      <c r="P17" s="18">
+      <c r="P17" s="15">
         <f t="shared" si="0"/>
         <v>707481.7</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="Q17" s="15">
         <f t="shared" si="0"/>
         <v>741835.7</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18">
         <v>2000</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="21">
+      <c r="D20" s="8"/>
+      <c r="E20" s="18">
         <v>2001</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="18">
         <v>2002</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="18">
         <v>2003</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="18">
         <v>2004</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="18">
         <v>2005</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="18">
         <v>2006</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K20" s="18">
         <v>2007</v>
       </c>
-      <c r="L20" s="21">
+      <c r="L20" s="18">
         <v>2008</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="18">
         <v>2009</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N20" s="18">
         <v>2010</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="18">
         <v>2011</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="19">
         <v>15</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="21">
         <v>92399</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="43">
         <f>C21+C22</f>
         <v>127577</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="21">
         <v>109578</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21" s="21">
         <v>133515</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="21">
         <v>162388</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="21">
         <v>171317</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I21" s="21">
         <v>204053</v>
       </c>
-      <c r="J21" s="24">
+      <c r="J21" s="21">
         <v>264566</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="21">
         <v>335547</v>
       </c>
-      <c r="L21" s="24">
+      <c r="L21" s="21">
         <v>457008</v>
       </c>
-      <c r="M21" s="24">
+      <c r="M21" s="21">
         <v>467249</v>
       </c>
-      <c r="N21" s="24">
+      <c r="N21" s="21">
         <v>468833</v>
       </c>
-      <c r="O21" s="24">
+      <c r="O21" s="21">
         <v>658497</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="A22" s="19">
         <v>16</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="21">
         <v>35178</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="24">
+      <c r="D22" s="43"/>
+      <c r="E22" s="21">
         <v>61307</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="21">
         <v>54631</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="21">
         <v>54245</v>
       </c>
-      <c r="H22" s="24">
+      <c r="H22" s="21">
         <v>51738</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I22" s="21">
         <v>59377</v>
       </c>
-      <c r="J22" s="24">
+      <c r="J22" s="21">
         <v>70506</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="21">
         <v>99672</v>
       </c>
-      <c r="L22" s="24">
+      <c r="L22" s="21">
         <v>124414</v>
       </c>
-      <c r="M22" s="24">
+      <c r="M22" s="21">
         <v>115360</v>
       </c>
-      <c r="N22" s="24">
+      <c r="N22" s="21">
         <v>112860</v>
       </c>
-      <c r="O22" s="24">
+      <c r="O22" s="21">
         <v>121284</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="19">
         <v>17</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C23" s="21">
         <v>67598</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="48">
         <f>SUM(C23:C25)</f>
         <v>106762</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <v>59131</v>
       </c>
-      <c r="F23" s="24">
+      <c r="F23" s="21">
         <v>68130</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="21">
         <v>73547</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="21">
         <v>85054</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="21">
         <v>93029</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J23" s="21">
         <v>103342</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="21">
         <v>111715</v>
       </c>
-      <c r="L23" s="24">
+      <c r="L23" s="21">
         <v>102965</v>
       </c>
-      <c r="M23" s="24">
+      <c r="M23" s="21">
         <v>121046</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23" s="21">
         <v>117985</v>
       </c>
-      <c r="O23" s="24">
+      <c r="O23" s="21">
         <v>161089</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="A24" s="19">
         <v>18</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="21">
         <v>24073</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="24">
+      <c r="D24" s="49"/>
+      <c r="E24" s="21">
         <v>27771</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="21">
         <v>28166</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="21">
         <v>31616</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="21">
         <v>30228</v>
       </c>
-      <c r="I24" s="24">
+      <c r="I24" s="21">
         <v>36806</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="21">
         <v>45369</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="21">
         <v>47105</v>
       </c>
-      <c r="L24" s="24">
+      <c r="L24" s="21">
         <v>43517</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="21">
         <v>47524</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="21">
         <v>60151</v>
       </c>
-      <c r="O24" s="24">
+      <c r="O24" s="21">
         <v>57298</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="19">
         <v>19</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="21">
         <v>15091</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="24">
+      <c r="D25" s="49"/>
+      <c r="E25" s="21">
         <v>17657</v>
       </c>
-      <c r="F25" s="24">
+      <c r="F25" s="21">
         <v>23775</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="21">
         <v>20870</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="21">
         <v>19228</v>
       </c>
-      <c r="I25" s="24">
+      <c r="I25" s="21">
         <v>22872</v>
       </c>
-      <c r="J25" s="24">
+      <c r="J25" s="21">
         <v>23472</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="21">
         <v>22238</v>
       </c>
-      <c r="L25" s="24">
+      <c r="L25" s="21">
         <v>35068</v>
       </c>
-      <c r="M25" s="24">
+      <c r="M25" s="21">
         <v>30136</v>
       </c>
-      <c r="N25" s="24">
+      <c r="N25" s="21">
         <v>32376</v>
       </c>
-      <c r="O25" s="24">
+      <c r="O25" s="21">
         <v>50096</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="19">
         <v>20</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="21">
         <v>35049</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="29">
         <f>C26</f>
         <v>35049</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <v>39704</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="21">
         <v>41781</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="21">
         <v>46736</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="21">
         <v>44254</v>
       </c>
-      <c r="I26" s="24">
+      <c r="I26" s="21">
         <v>44755</v>
       </c>
-      <c r="J26" s="24">
+      <c r="J26" s="21">
         <v>38205</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="21">
         <v>47749</v>
       </c>
-      <c r="L26" s="24">
+      <c r="L26" s="21">
         <v>45248</v>
       </c>
-      <c r="M26" s="24">
+      <c r="M26" s="21">
         <v>36830</v>
       </c>
-      <c r="N26" s="24">
+      <c r="N26" s="21">
         <v>37443</v>
       </c>
-      <c r="O26" s="24">
+      <c r="O26" s="21">
         <v>39566</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="A27" s="19">
         <v>21</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="21">
         <v>37027</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="50">
         <f>SUM(C27:C28)</f>
         <v>48633</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>48441</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="21">
         <v>65898</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="21">
         <v>56191</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="21">
         <v>56486</v>
       </c>
-      <c r="I27" s="24">
+      <c r="I27" s="21">
         <v>68226</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="21">
         <v>71959</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="21">
         <v>91756</v>
       </c>
-      <c r="L27" s="24">
+      <c r="L27" s="21">
         <v>97219</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27" s="21">
         <v>107149</v>
       </c>
-      <c r="N27" s="24">
+      <c r="N27" s="21">
         <v>114388</v>
       </c>
-      <c r="O27" s="24">
+      <c r="O27" s="21">
         <v>130165</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
+      <c r="A28" s="19">
         <v>22</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="21">
         <v>11606</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="24">
+      <c r="D28" s="51"/>
+      <c r="E28" s="21">
         <v>3757</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="21">
         <v>6272</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="21">
         <v>7484</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="21">
         <v>12174</v>
       </c>
-      <c r="I28" s="24">
+      <c r="I28" s="21">
         <v>14156</v>
       </c>
-      <c r="J28" s="24">
+      <c r="J28" s="21">
         <v>12955</v>
       </c>
-      <c r="K28" s="24">
+      <c r="K28" s="21">
         <v>15581</v>
       </c>
-      <c r="L28" s="24">
+      <c r="L28" s="21">
         <v>13959</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28" s="21">
         <v>20614</v>
       </c>
-      <c r="N28" s="24">
+      <c r="N28" s="21">
         <v>13806</v>
       </c>
-      <c r="O28" s="24">
+      <c r="O28" s="21">
         <v>24064</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="A29" s="19">
         <v>23</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="21">
         <v>1492</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="24">
+      <c r="D29" s="8"/>
+      <c r="E29" s="21">
         <v>342</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="21">
         <v>786</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="21">
         <v>1715</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="21">
         <v>1421</v>
       </c>
-      <c r="I29" s="24">
+      <c r="I29" s="21">
         <v>2023</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="21">
         <v>7893</v>
       </c>
-      <c r="K29" s="24">
+      <c r="K29" s="21">
         <v>7527</v>
       </c>
-      <c r="L29" s="24">
+      <c r="L29" s="21">
         <v>11040</v>
       </c>
-      <c r="M29" s="24">
+      <c r="M29" s="21">
         <v>7976</v>
       </c>
-      <c r="N29" s="24">
+      <c r="N29" s="21">
         <v>7168</v>
       </c>
-      <c r="O29" s="24">
+      <c r="O29" s="21">
         <v>5063</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="11">
         <v>24</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="9">
         <v>61388</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="43">
         <f>C30+C31</f>
         <v>95893</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="21">
         <v>86376</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="21">
         <v>90492</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="21">
         <v>90286</v>
       </c>
-      <c r="H30" s="24">
+      <c r="H30" s="21">
         <v>92767</v>
       </c>
-      <c r="I30" s="24">
+      <c r="I30" s="21">
         <v>110065</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="21">
         <v>147580</v>
       </c>
-      <c r="K30" s="24">
+      <c r="K30" s="21">
         <v>173134</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="21">
         <v>266230</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="21">
         <v>314739</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="21">
         <v>311806</v>
       </c>
-      <c r="O30" s="24">
+      <c r="O30" s="21">
         <v>359715</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="11">
         <v>25</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="9">
         <v>34505</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="24">
+      <c r="D31" s="44"/>
+      <c r="E31" s="21">
         <v>33435</v>
       </c>
-      <c r="F31" s="24">
+      <c r="F31" s="21">
         <v>41909</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="21">
         <v>45158</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H31" s="21">
         <v>67838</v>
       </c>
-      <c r="I31" s="24">
+      <c r="I31" s="21">
         <v>97521</v>
       </c>
-      <c r="J31" s="24">
+      <c r="J31" s="21">
         <v>99995</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="21">
         <v>105798</v>
       </c>
-      <c r="L31" s="24">
+      <c r="L31" s="21">
         <v>158372</v>
       </c>
-      <c r="M31" s="24">
+      <c r="M31" s="21">
         <v>142125</v>
       </c>
-      <c r="N31" s="24">
+      <c r="N31" s="21">
         <v>251502</v>
       </c>
-      <c r="O31" s="24">
+      <c r="O31" s="21">
         <v>284834</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
+      <c r="A32" s="19">
         <v>26</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="21">
         <v>18684</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="24">
+      <c r="D32" s="8"/>
+      <c r="E32" s="21">
         <v>23768</v>
       </c>
-      <c r="F32" s="24">
+      <c r="F32" s="21">
         <v>23815</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="21">
         <v>25578</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="21">
         <v>36604</v>
       </c>
-      <c r="I32" s="24">
+      <c r="I32" s="21">
         <v>37284</v>
       </c>
-      <c r="J32" s="24">
+      <c r="J32" s="21">
         <v>39659</v>
       </c>
-      <c r="K32" s="24">
+      <c r="K32" s="21">
         <v>44500</v>
       </c>
-      <c r="L32" s="24">
+      <c r="L32" s="21">
         <v>53369</v>
       </c>
-      <c r="M32" s="24">
+      <c r="M32" s="21">
         <v>54410</v>
       </c>
-      <c r="N32" s="24">
+      <c r="N32" s="21">
         <v>52751</v>
       </c>
-      <c r="O32" s="24">
+      <c r="O32" s="21">
         <v>65051</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
+      <c r="A33" s="19">
         <v>27</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="21">
         <v>30893</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="24">
+      <c r="D33" s="8"/>
+      <c r="E33" s="21">
         <v>45124</v>
       </c>
-      <c r="F33" s="24">
+      <c r="F33" s="21">
         <v>43278</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="21">
         <v>49664</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="21">
         <v>62229</v>
       </c>
-      <c r="I33" s="24">
+      <c r="I33" s="21">
         <v>79920</v>
       </c>
-      <c r="J33" s="24">
+      <c r="J33" s="21">
         <v>81762</v>
       </c>
-      <c r="K33" s="24">
+      <c r="K33" s="21">
         <v>108285</v>
       </c>
-      <c r="L33" s="24">
+      <c r="L33" s="21">
         <v>112776</v>
       </c>
-      <c r="M33" s="24">
+      <c r="M33" s="21">
         <v>102743</v>
       </c>
-      <c r="N33" s="24">
+      <c r="N33" s="21">
         <v>136122</v>
       </c>
-      <c r="O33" s="24">
+      <c r="O33" s="21">
         <v>90784</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+      <c r="A34" s="11">
         <v>28</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="9">
         <v>18663</v>
       </c>
-      <c r="D34" s="41">
+      <c r="D34" s="43">
         <f>C34+C35</f>
         <v>24401</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="21">
         <v>11844</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="21">
         <v>102004</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="21">
         <v>20105</v>
       </c>
-      <c r="H34" s="24">
+      <c r="H34" s="21">
         <v>27376</v>
       </c>
-      <c r="I34" s="24">
+      <c r="I34" s="21">
         <v>24192</v>
       </c>
-      <c r="J34" s="24">
+      <c r="J34" s="21">
         <v>32200</v>
       </c>
-      <c r="K34" s="24">
+      <c r="K34" s="21">
         <v>41266</v>
       </c>
-      <c r="L34" s="24">
+      <c r="L34" s="21">
         <v>49619</v>
       </c>
-      <c r="M34" s="24">
+      <c r="M34" s="21">
         <v>64112</v>
       </c>
-      <c r="N34" s="24">
+      <c r="N34" s="21">
         <v>68545</v>
       </c>
-      <c r="O34" s="24">
+      <c r="O34" s="21">
         <v>79466</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+      <c r="A35" s="11">
         <v>29</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="9">
         <v>5738</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="24">
+      <c r="D35" s="44"/>
+      <c r="E35" s="21">
         <v>37324</v>
       </c>
-      <c r="F35" s="24">
+      <c r="F35" s="21">
         <v>13070</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="21">
         <v>12479</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="21">
         <v>14141</v>
       </c>
-      <c r="I35" s="24">
+      <c r="I35" s="21">
         <v>16832</v>
       </c>
-      <c r="J35" s="24">
+      <c r="J35" s="21">
         <v>24455</v>
       </c>
-      <c r="K35" s="24">
+      <c r="K35" s="21">
         <v>21356</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L35" s="21">
         <v>32504</v>
       </c>
-      <c r="M35" s="24">
+      <c r="M35" s="21">
         <v>31950</v>
       </c>
-      <c r="N35" s="24">
+      <c r="N35" s="21">
         <v>61258</v>
       </c>
-      <c r="O35" s="24">
+      <c r="O35" s="21">
         <v>37462</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="22">
+      <c r="A36" s="19">
         <v>30</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="21">
         <v>26</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="24">
+      <c r="D36" s="8"/>
+      <c r="E36" s="21">
         <v>28</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="21">
         <v>47</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="21">
         <v>87</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="21">
         <v>85</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="21">
         <v>1762</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="21">
         <v>165</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="21">
         <v>274</v>
       </c>
-      <c r="L36" s="24">
+      <c r="L36" s="21">
         <v>531</v>
       </c>
-      <c r="M36" s="24">
+      <c r="M36" s="21">
         <v>319</v>
       </c>
-      <c r="N36" s="24">
+      <c r="N36" s="21">
         <v>351</v>
       </c>
-      <c r="O36" s="24">
+      <c r="O36" s="21">
         <v>2022</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
+      <c r="A37" s="19">
         <v>31</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="21">
         <v>20787</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="24">
+      <c r="D37" s="8"/>
+      <c r="E37" s="21">
         <v>17039</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="21">
         <v>14769</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="21">
         <v>17157</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="21">
         <v>33437</v>
       </c>
-      <c r="I37" s="24">
+      <c r="I37" s="21">
         <v>25534</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="21">
         <v>31863</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="21">
         <v>33803</v>
       </c>
-      <c r="L37" s="24">
+      <c r="L37" s="21">
         <v>51427</v>
       </c>
-      <c r="M37" s="24">
+      <c r="M37" s="21">
         <v>49940</v>
       </c>
-      <c r="N37" s="24">
+      <c r="N37" s="21">
         <v>56098</v>
       </c>
-      <c r="O37" s="24">
+      <c r="O37" s="21">
         <v>60091</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
+      <c r="A38" s="19">
         <v>32</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="21">
         <v>43515</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="24">
+      <c r="D38" s="8"/>
+      <c r="E38" s="21">
         <v>26157</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="21">
         <v>32262</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="21">
         <v>39959</v>
       </c>
-      <c r="H38" s="24">
+      <c r="H38" s="21">
         <v>77344</v>
       </c>
-      <c r="I38" s="24">
+      <c r="I38" s="21">
         <v>28197</v>
       </c>
-      <c r="J38" s="24">
+      <c r="J38" s="21">
         <v>46441</v>
       </c>
-      <c r="K38" s="24">
+      <c r="K38" s="21">
         <v>45711</v>
       </c>
-      <c r="L38" s="24">
+      <c r="L38" s="21">
         <v>40248</v>
       </c>
-      <c r="M38" s="24">
+      <c r="M38" s="21">
         <v>55043</v>
       </c>
-      <c r="N38" s="24">
+      <c r="N38" s="21">
         <v>50151</v>
       </c>
-      <c r="O38" s="24">
+      <c r="O38" s="21">
         <v>53785</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
+      <c r="A39" s="19">
         <v>33</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="21">
         <v>2088</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="24">
+      <c r="D39" s="8"/>
+      <c r="E39" s="21">
         <v>1596</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="21">
         <v>1154</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="21">
         <v>1704</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="21">
         <v>1615</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="21">
         <v>2382</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="21">
         <v>4832</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="21">
         <v>4188</v>
       </c>
-      <c r="L39" s="24">
+      <c r="L39" s="21">
         <v>3236</v>
       </c>
-      <c r="M39" s="24">
+      <c r="M39" s="21">
         <v>2747</v>
       </c>
-      <c r="N39" s="24">
+      <c r="N39" s="21">
         <v>3873</v>
       </c>
-      <c r="O39" s="24">
+      <c r="O39" s="21">
         <v>2583</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="22">
+      <c r="A40" s="19">
         <v>34</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="21">
         <v>27450</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="24">
+      <c r="D40" s="8"/>
+      <c r="E40" s="21">
         <v>26320</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F40" s="21">
         <v>52536</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="21">
         <v>27885</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="21">
         <v>49506</v>
       </c>
-      <c r="I40" s="24">
+      <c r="I40" s="21">
         <v>63249</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="21">
         <v>69848</v>
       </c>
-      <c r="K40" s="24">
+      <c r="K40" s="21">
         <v>71569</v>
       </c>
-      <c r="L40" s="24">
+      <c r="L40" s="21">
         <v>87639</v>
       </c>
-      <c r="M40" s="24">
+      <c r="M40" s="21">
         <v>95277</v>
       </c>
-      <c r="N40" s="24">
+      <c r="N40" s="21">
         <v>125027</v>
       </c>
-      <c r="O40" s="24">
+      <c r="O40" s="21">
         <v>201155</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="A41" s="19">
         <v>35</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="21">
         <v>33765</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="24">
+      <c r="D41" s="8"/>
+      <c r="E41" s="21">
         <v>29268</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="21">
         <v>26849</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="21">
         <v>37667</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="21">
         <v>32354</v>
       </c>
-      <c r="I41" s="24">
+      <c r="I41" s="21">
         <v>36220</v>
       </c>
-      <c r="J41" s="24">
+      <c r="J41" s="21">
         <v>46245</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="21">
         <v>72294</v>
       </c>
-      <c r="L41" s="24">
+      <c r="L41" s="21">
         <v>90425</v>
       </c>
-      <c r="M41" s="24">
+      <c r="M41" s="21">
         <v>99600</v>
       </c>
-      <c r="N41" s="24">
+      <c r="N41" s="21">
         <v>86990</v>
       </c>
-      <c r="O41" s="24">
+      <c r="O41" s="21">
         <v>88603</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
+      <c r="A42" s="19">
         <v>36</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="21">
         <v>11939</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="24">
+      <c r="D42" s="8"/>
+      <c r="E42" s="21">
         <v>13233</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="21">
         <v>17128</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="21">
         <v>16053</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="21">
         <v>18518</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="21">
         <v>19970</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="21">
         <v>27921</v>
       </c>
-      <c r="K42" s="24">
+      <c r="K42" s="21">
         <v>44157</v>
       </c>
-      <c r="L42" s="24">
+      <c r="L42" s="21">
         <v>39647</v>
       </c>
-      <c r="M42" s="24">
+      <c r="M42" s="21">
         <v>32629</v>
       </c>
-      <c r="N42" s="24">
+      <c r="N42" s="21">
         <v>38467</v>
       </c>
-      <c r="O42" s="24">
+      <c r="O42" s="21">
         <v>45376</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="25">
+      <c r="B43" s="24"/>
+      <c r="C43" s="22">
         <v>628954</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="25">
+      <c r="D43" s="8"/>
+      <c r="E43" s="22">
         <v>719200</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="22">
         <v>882267</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="22">
         <v>838574</v>
       </c>
-      <c r="H43" s="25">
+      <c r="H43" s="22">
         <v>985714</v>
       </c>
-      <c r="I43" s="26">
+      <c r="I43" s="23">
         <v>1088425</v>
       </c>
-      <c r="J43" s="26">
+      <c r="J43" s="23">
         <v>1291233</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K43" s="23">
         <v>1545225</v>
       </c>
-      <c r="L43" s="26">
+      <c r="L43" s="23">
         <v>1916461</v>
       </c>
-      <c r="M43" s="26">
+      <c r="M43" s="23">
         <v>1999518</v>
       </c>
-      <c r="N43" s="26">
+      <c r="N43" s="23">
         <v>2207951</v>
       </c>
-      <c r="O43" s="26">
+      <c r="O43" s="23">
         <v>2618049</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="47"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="47"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D46" s="28">
+      <c r="D46" s="25">
         <f>SUM(D21:D42)</f>
         <v>438315</v>
       </c>
@@ -4945,13 +5137,144 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDB59F0-D6B3-4A6B-A133-7B17C332CA6B}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="32">
+        <v>6015</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="32">
+        <v>9868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="32">
+        <v>4847</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>2003</v>
+      </c>
+      <c r="B5" s="32">
+        <v>5782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>2004</v>
+      </c>
+      <c r="B6" s="32">
+        <v>6952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="32">
+        <v>7599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>2006</v>
+      </c>
+      <c r="B8" s="33">
+        <v>10507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>2007</v>
+      </c>
+      <c r="B9" s="33">
+        <v>9972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>2008</v>
+      </c>
+      <c r="B10" s="33">
+        <v>10508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>2009</v>
+      </c>
+      <c r="B11" s="33">
+        <v>24358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="33">
+        <v>12994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="32">
+        <v>25442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0A275E-95A3-45C9-8796-8D4F4C7E0B61}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
added revision on AKSI MITIGASI ENERGI + BIAYA 19 NOV.xlsx. added  revision on HEESI data recap.
</commit_message>
<xml_diff>
--- a/Industri/Industri.xlsx
+++ b/Industri/Industri.xlsx
@@ -1,42 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\System Dynamics\Github\system_dynamics_reference\Industri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9CB069-B369-4A98-8769-2FFD4B20D77A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5E66FD-42BE-4D02-8850-3704A66B0390}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data industri" sheetId="1" r:id="rId1"/>
-    <sheet name="Pertanian" sheetId="6" r:id="rId2"/>
-    <sheet name="Nilai Tambah" sheetId="2" r:id="rId3"/>
-    <sheet name="PDB Industri Harga 2000" sheetId="4" r:id="rId4"/>
-    <sheet name="Pengeluaran untuk Naker" sheetId="3" r:id="rId5"/>
-    <sheet name="Jabar" sheetId="5" r:id="rId6"/>
+    <sheet name="PDB" sheetId="7" r:id="rId1"/>
+    <sheet name="Semen" sheetId="8" r:id="rId2"/>
+    <sheet name="Besi Baja" sheetId="9" r:id="rId3"/>
+    <sheet name="data industri" sheetId="1" r:id="rId4"/>
+    <sheet name="Pertanian" sheetId="6" r:id="rId5"/>
+    <sheet name="Nilai Tambah" sheetId="2" r:id="rId6"/>
+    <sheet name="PDB Industri Harga 2000" sheetId="4" r:id="rId7"/>
+    <sheet name="Pengeluaran untuk Naker" sheetId="3" r:id="rId8"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
   <si>
     <t>Tahun</t>
   </si>
@@ -189,6 +186,204 @@
   </si>
   <si>
     <t>Produksi (ton)</t>
+  </si>
+  <si>
+    <t>B, Pertambangan dan Penggalian</t>
+  </si>
+  <si>
+    <t>1, Pertambangan Minyak, Gas dan Panas Bumi</t>
+  </si>
+  <si>
+    <t>2, Pertambangan Batubara dan Lignit</t>
+  </si>
+  <si>
+    <t>3, Pertambangan Bijih Logam</t>
+  </si>
+  <si>
+    <t>4, Pertambangan dan Penggalian Lainnya</t>
+  </si>
+  <si>
+    <t>C, Industri Pengolahan</t>
+  </si>
+  <si>
+    <t>1, Industri Batubara dan Pengilangan Migas</t>
+  </si>
+  <si>
+    <t>Industri Pengolahan Non Migas</t>
+  </si>
+  <si>
+    <t>1, Industri Makanan dan Minuman</t>
+  </si>
+  <si>
+    <t>2, Industri Pengolahan Tembakau</t>
+  </si>
+  <si>
+    <t>3, Industri Tekstil dan Pakaian Jadi</t>
+  </si>
+  <si>
+    <t>4, Industri Kulit, Barang dari Kulit dan Alas Kaki</t>
+  </si>
+  <si>
+    <t>5, Industri Kayu, Barang dari Kayu dan Gabus dan Barang Anyaman dari Bambu, Rotan dan Sejenisnya</t>
+  </si>
+  <si>
+    <t>6, Industri Kertas dan Barang dari Kertas; Percetakan dan Reproduksi Media Rekaman</t>
+  </si>
+  <si>
+    <t>7, Industri Kimia, Farmasi dan Obat Tradisional</t>
+  </si>
+  <si>
+    <t>8, Industri Karet, Barang dari Karet dan Plastik</t>
+  </si>
+  <si>
+    <t>9, Industri Barang Galian bukan Logam</t>
+  </si>
+  <si>
+    <t>10, Industri Logam Dasar</t>
+  </si>
+  <si>
+    <t>11, Industri Barang Logam; Komputer, Barang Elektronik, Optik; dan Peralatan Listrik</t>
+  </si>
+  <si>
+    <t>12, Industri Mesin dan Perlengkapan</t>
+  </si>
+  <si>
+    <t>13, Industri Alat Angkutan</t>
+  </si>
+  <si>
+    <t>14, Industri Furnitur</t>
+  </si>
+  <si>
+    <t>15, Industri Pengolahan Lainnya; Jasa Reparasi dan Pemasangan Mesin dan Peralatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Urea </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Fosfat/SP-36 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. ZA/AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. NPK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. ZK(K2SO4) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Organik </t>
+  </si>
+  <si>
+    <t>Jan-Sept 2020</t>
+  </si>
+  <si>
+    <t>Total Produksi</t>
+  </si>
+  <si>
+    <t>Produksi Pupuk (ton/tahun)</t>
+  </si>
+  <si>
+    <t>Produksi Semen (ton/Tahun)</t>
+  </si>
+  <si>
+    <t>SINAR TAMBANG ARTHA LESTARI, PT</t>
+  </si>
+  <si>
+    <t>SEMEN TONASA, PT</t>
+  </si>
+  <si>
+    <t>SEMEN PADANG, PT</t>
+  </si>
+  <si>
+    <t>SEMEN KUPANG, PT</t>
+  </si>
+  <si>
+    <t>SEMEN JAWA, PT</t>
+  </si>
+  <si>
+    <t>SEMEN GRESIK, PT</t>
+  </si>
+  <si>
+    <t>SEMEN BOSOWA MAROS, PT</t>
+  </si>
+  <si>
+    <t>SEMEN BATURAJA, PT</t>
+  </si>
+  <si>
+    <t>LAFARGE HOLCIM INDONESIA, PT</t>
+  </si>
+  <si>
+    <t>JUI SHIN INDONESIA, PT</t>
+  </si>
+  <si>
+    <t>INDOCEMENT TUNGGAL PRAKARSA, PT</t>
+  </si>
+  <si>
+    <t>CONCH CEMENT INDONESIA, PT</t>
+  </si>
+  <si>
+    <t>CEMINDO GEMILANG, PT</t>
+  </si>
+  <si>
+    <t>Proyeksi Pertumbuhan Demand Baja Nasional (Ton)</t>
+  </si>
+  <si>
+    <t>2015-2020</t>
+  </si>
+  <si>
+    <t>% Pertumbuhan Rata-Rata</t>
+  </si>
+  <si>
+    <t>Proyeksi 2020</t>
+  </si>
+  <si>
+    <t>HRC</t>
+  </si>
+  <si>
+    <t>PLATE</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>BAJA TULANGAN BETON</t>
+  </si>
+  <si>
+    <t>BAJA PROFIL</t>
+  </si>
+  <si>
+    <t>WIRE ROD</t>
+  </si>
+  <si>
+    <t>STEEL PIPE</t>
+  </si>
+  <si>
+    <t>COATED SHEET</t>
+  </si>
+  <si>
+    <t>TINPLATE</t>
+  </si>
+  <si>
+    <t>KAWAT</t>
+  </si>
+  <si>
+    <t>PAKU</t>
+  </si>
+  <si>
+    <t>MUR BAUT</t>
+  </si>
+  <si>
+    <t>Ekstrapolasi Demand Baja Nasional</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Tren 2013-2020</t>
+  </si>
+  <si>
+    <t>Tren 2013 - 2000</t>
   </si>
 </sst>
 </file>
@@ -817,7 +1012,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1078,6 +1273,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1176,7 +1386,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -1279,6 +1489,36 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="94" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="94" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="94" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="48" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,6 +1560,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="95">
@@ -1694,6 +1940,2186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2118F3-97E8-43CE-9774-E271B08C95F9}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="91.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="17">
+        <v>2010</v>
+      </c>
+      <c r="C1" s="17">
+        <v>2011</v>
+      </c>
+      <c r="D1" s="17">
+        <v>2012</v>
+      </c>
+      <c r="E1" s="17">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="17">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="17">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="17">
+        <v>2016</v>
+      </c>
+      <c r="I1" s="17">
+        <v>2017</v>
+      </c>
+      <c r="J1" s="17">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="17">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="38">
+        <v>718128.6</v>
+      </c>
+      <c r="C2" s="38">
+        <v>748956.3</v>
+      </c>
+      <c r="D2" s="38">
+        <v>771561.6</v>
+      </c>
+      <c r="E2" s="38">
+        <v>791054.4</v>
+      </c>
+      <c r="F2" s="38">
+        <v>794489.5</v>
+      </c>
+      <c r="G2" s="38">
+        <v>767327.2</v>
+      </c>
+      <c r="H2" s="38">
+        <v>774593.1</v>
+      </c>
+      <c r="I2" s="38">
+        <v>779678.4</v>
+      </c>
+      <c r="J2" s="38">
+        <v>796505</v>
+      </c>
+      <c r="K2" s="38">
+        <v>806206.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>336169.7</v>
+      </c>
+      <c r="C3">
+        <v>335737.1</v>
+      </c>
+      <c r="D3">
+        <v>323632.40000000002</v>
+      </c>
+      <c r="E3">
+        <v>313328.09999999998</v>
+      </c>
+      <c r="F3">
+        <v>307161.7</v>
+      </c>
+      <c r="G3">
+        <v>307325.8</v>
+      </c>
+      <c r="H3">
+        <v>313743.90000000002</v>
+      </c>
+      <c r="I3">
+        <v>302653</v>
+      </c>
+      <c r="J3">
+        <v>298420.09999999998</v>
+      </c>
+      <c r="K3">
+        <v>289980.09999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>160732.5</v>
+      </c>
+      <c r="C4">
+        <v>199244</v>
+      </c>
+      <c r="D4">
+        <v>230589.2</v>
+      </c>
+      <c r="E4">
+        <v>247594.6</v>
+      </c>
+      <c r="F4">
+        <v>251073.6</v>
+      </c>
+      <c r="G4">
+        <v>232725.3</v>
+      </c>
+      <c r="H4">
+        <v>223098.6</v>
+      </c>
+      <c r="I4">
+        <v>226478.9</v>
+      </c>
+      <c r="J4">
+        <v>235561.4</v>
+      </c>
+      <c r="K4">
+        <v>259598.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>109244.2</v>
+      </c>
+      <c r="C5">
+        <v>95413.7</v>
+      </c>
+      <c r="D5">
+        <v>91614.5</v>
+      </c>
+      <c r="E5">
+        <v>98608.6</v>
+      </c>
+      <c r="F5">
+        <v>98257.9</v>
+      </c>
+      <c r="G5">
+        <v>87702.9</v>
+      </c>
+      <c r="H5">
+        <v>89303.2</v>
+      </c>
+      <c r="I5">
+        <v>95150.399999999994</v>
+      </c>
+      <c r="J5">
+        <v>103719.4</v>
+      </c>
+      <c r="K5">
+        <v>88003.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>111982.2</v>
+      </c>
+      <c r="C6">
+        <v>118561.5</v>
+      </c>
+      <c r="D6">
+        <v>125725.5</v>
+      </c>
+      <c r="E6">
+        <v>131523.1</v>
+      </c>
+      <c r="F6">
+        <v>137996.29999999999</v>
+      </c>
+      <c r="G6">
+        <v>139573.20000000001</v>
+      </c>
+      <c r="H6">
+        <v>148447.4</v>
+      </c>
+      <c r="I6">
+        <v>155396.1</v>
+      </c>
+      <c r="J6">
+        <v>158804.1</v>
+      </c>
+      <c r="K6">
+        <v>168624.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="38">
+        <v>1512760.8</v>
+      </c>
+      <c r="C7" s="38">
+        <v>1607452</v>
+      </c>
+      <c r="D7" s="38">
+        <v>1697787.2</v>
+      </c>
+      <c r="E7" s="38">
+        <v>1771961.9</v>
+      </c>
+      <c r="F7" s="38">
+        <v>1854256.7</v>
+      </c>
+      <c r="G7" s="38">
+        <v>1934533.2</v>
+      </c>
+      <c r="H7" s="38">
+        <v>2016876.9</v>
+      </c>
+      <c r="I7" s="38">
+        <v>2103466.1</v>
+      </c>
+      <c r="J7" s="38">
+        <v>2193368.4</v>
+      </c>
+      <c r="K7" s="38">
+        <v>2276682.7999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>233822.2</v>
+      </c>
+      <c r="C8">
+        <v>233051.9</v>
+      </c>
+      <c r="D8">
+        <v>227456.1</v>
+      </c>
+      <c r="E8">
+        <v>221449.9</v>
+      </c>
+      <c r="F8">
+        <v>216750.8</v>
+      </c>
+      <c r="G8">
+        <v>214312</v>
+      </c>
+      <c r="H8">
+        <v>220392.1</v>
+      </c>
+      <c r="I8">
+        <v>219849.4</v>
+      </c>
+      <c r="J8">
+        <v>219831.8</v>
+      </c>
+      <c r="K8">
+        <v>217417.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="38">
+        <v>1278938.6000000001</v>
+      </c>
+      <c r="C9" s="38">
+        <v>1374400.1</v>
+      </c>
+      <c r="D9" s="38">
+        <v>1470331.1</v>
+      </c>
+      <c r="E9" s="38">
+        <v>1550512</v>
+      </c>
+      <c r="F9" s="38">
+        <v>1637505.9</v>
+      </c>
+      <c r="G9" s="38">
+        <v>1720221.2</v>
+      </c>
+      <c r="H9" s="38">
+        <v>1796484.8</v>
+      </c>
+      <c r="I9" s="38">
+        <v>1883616.7</v>
+      </c>
+      <c r="J9" s="38">
+        <v>1973536.6</v>
+      </c>
+      <c r="K9" s="38">
+        <v>2059265.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>360443.1</v>
+      </c>
+      <c r="C10">
+        <v>400003.7</v>
+      </c>
+      <c r="D10">
+        <v>441341.7</v>
+      </c>
+      <c r="E10">
+        <v>459283</v>
+      </c>
+      <c r="F10">
+        <v>502856.2</v>
+      </c>
+      <c r="G10">
+        <v>540756.4</v>
+      </c>
+      <c r="H10">
+        <v>585786.30000000005</v>
+      </c>
+      <c r="I10">
+        <v>639834.4</v>
+      </c>
+      <c r="J10">
+        <v>690462.5</v>
+      </c>
+      <c r="K10">
+        <v>744170.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>67249.399999999994</v>
+      </c>
+      <c r="C11">
+        <v>67096.800000000003</v>
+      </c>
+      <c r="D11">
+        <v>73011.399999999994</v>
+      </c>
+      <c r="E11">
+        <v>72814</v>
+      </c>
+      <c r="F11">
+        <v>78878.7</v>
+      </c>
+      <c r="G11">
+        <v>83798.7</v>
+      </c>
+      <c r="H11">
+        <v>85119.7</v>
+      </c>
+      <c r="I11">
+        <v>84572.4</v>
+      </c>
+      <c r="J11">
+        <v>87548.7</v>
+      </c>
+      <c r="K11">
+        <v>90486.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>96306.9</v>
+      </c>
+      <c r="C12">
+        <v>102561.1</v>
+      </c>
+      <c r="D12">
+        <v>108753.60000000001</v>
+      </c>
+      <c r="E12">
+        <v>115913.1</v>
+      </c>
+      <c r="F12">
+        <v>117723.4</v>
+      </c>
+      <c r="G12">
+        <v>112078.9</v>
+      </c>
+      <c r="H12">
+        <v>111978.2</v>
+      </c>
+      <c r="I12">
+        <v>116261.6</v>
+      </c>
+      <c r="J12">
+        <v>126406.8</v>
+      </c>
+      <c r="K12">
+        <v>145804.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>19697.2</v>
+      </c>
+      <c r="C13">
+        <v>21852.3</v>
+      </c>
+      <c r="D13">
+        <v>20665.3</v>
+      </c>
+      <c r="E13">
+        <v>21745.7</v>
+      </c>
+      <c r="F13">
+        <v>22967.7</v>
+      </c>
+      <c r="G13">
+        <v>23879.200000000001</v>
+      </c>
+      <c r="H13">
+        <v>25875.3</v>
+      </c>
+      <c r="I13">
+        <v>26449</v>
+      </c>
+      <c r="J13">
+        <v>28941.7</v>
+      </c>
+      <c r="K13">
+        <v>28654.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>56775.1</v>
+      </c>
+      <c r="C14">
+        <v>55230.9</v>
+      </c>
+      <c r="D14">
+        <v>54786.9</v>
+      </c>
+      <c r="E14">
+        <v>58180.6</v>
+      </c>
+      <c r="F14">
+        <v>61742.5</v>
+      </c>
+      <c r="G14">
+        <v>60735.4</v>
+      </c>
+      <c r="H14">
+        <v>61790.6</v>
+      </c>
+      <c r="I14">
+        <v>61870.400000000001</v>
+      </c>
+      <c r="J14">
+        <v>62337.3</v>
+      </c>
+      <c r="K14">
+        <v>59498.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15">
+        <v>67984.800000000003</v>
+      </c>
+      <c r="C15">
+        <v>70631.600000000006</v>
+      </c>
+      <c r="D15">
+        <v>68590.399999999994</v>
+      </c>
+      <c r="E15">
+        <v>68229.399999999994</v>
+      </c>
+      <c r="F15">
+        <v>70670.100000000006</v>
+      </c>
+      <c r="G15">
+        <v>70556.800000000003</v>
+      </c>
+      <c r="H15">
+        <v>72399.899999999994</v>
+      </c>
+      <c r="I15">
+        <v>72640.600000000006</v>
+      </c>
+      <c r="J15">
+        <v>73681.600000000006</v>
+      </c>
+      <c r="K15">
+        <v>80211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>114332.4</v>
+      </c>
+      <c r="C16">
+        <v>124230.7</v>
+      </c>
+      <c r="D16">
+        <v>140101.79999999999</v>
+      </c>
+      <c r="E16">
+        <v>147248.6</v>
+      </c>
+      <c r="F16">
+        <v>153191.9</v>
+      </c>
+      <c r="G16">
+        <v>164843</v>
+      </c>
+      <c r="H16">
+        <v>174469.8</v>
+      </c>
+      <c r="I16">
+        <v>182380.2</v>
+      </c>
+      <c r="J16">
+        <v>179791.9</v>
+      </c>
+      <c r="K16">
+        <v>195040.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>66763</v>
+      </c>
+      <c r="C17">
+        <v>68152.600000000006</v>
+      </c>
+      <c r="D17">
+        <v>73307.399999999994</v>
+      </c>
+      <c r="E17">
+        <v>71945.7</v>
+      </c>
+      <c r="F17">
+        <v>72777.3</v>
+      </c>
+      <c r="G17">
+        <v>76442.100000000006</v>
+      </c>
+      <c r="H17">
+        <v>69940.899999999994</v>
+      </c>
+      <c r="I17">
+        <v>71666.8</v>
+      </c>
+      <c r="J17">
+        <v>76627.8</v>
+      </c>
+      <c r="K17">
+        <v>72398.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>50948.3</v>
+      </c>
+      <c r="C18">
+        <v>54909.8</v>
+      </c>
+      <c r="D18">
+        <v>59252.4</v>
+      </c>
+      <c r="E18">
+        <v>61228.7</v>
+      </c>
+      <c r="F18">
+        <v>62706.8</v>
+      </c>
+      <c r="G18">
+        <v>66485.2</v>
+      </c>
+      <c r="H18">
+        <v>70118.7</v>
+      </c>
+      <c r="I18">
+        <v>69512.899999999994</v>
+      </c>
+      <c r="J18">
+        <v>71424.399999999994</v>
+      </c>
+      <c r="K18">
+        <v>70690.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>54471.5</v>
+      </c>
+      <c r="C19">
+        <v>61859.7</v>
+      </c>
+      <c r="D19">
+        <v>60888.7</v>
+      </c>
+      <c r="E19">
+        <v>67972.399999999994</v>
+      </c>
+      <c r="F19">
+        <v>72059.100000000006</v>
+      </c>
+      <c r="G19">
+        <v>76532.100000000006</v>
+      </c>
+      <c r="H19">
+        <v>77293</v>
+      </c>
+      <c r="I19">
+        <v>81832.600000000006</v>
+      </c>
+      <c r="J19">
+        <v>89188.6</v>
+      </c>
+      <c r="K19">
+        <v>91716.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20">
+        <v>130750.5</v>
+      </c>
+      <c r="C20">
+        <v>142245</v>
+      </c>
+      <c r="D20">
+        <v>158803.5</v>
+      </c>
+      <c r="E20">
+        <v>173452.4</v>
+      </c>
+      <c r="F20">
+        <v>178544.2</v>
+      </c>
+      <c r="G20">
+        <v>192528</v>
+      </c>
+      <c r="H20">
+        <v>200860.9</v>
+      </c>
+      <c r="I20">
+        <v>206469.3</v>
+      </c>
+      <c r="J20">
+        <v>205216.8</v>
+      </c>
+      <c r="K20">
+        <v>204172.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>23767.200000000001</v>
+      </c>
+      <c r="C21">
+        <v>25794.5</v>
+      </c>
+      <c r="D21">
+        <v>25436.7</v>
+      </c>
+      <c r="E21">
+        <v>24163.8</v>
+      </c>
+      <c r="F21">
+        <v>26259.7</v>
+      </c>
+      <c r="G21">
+        <v>28250.5</v>
+      </c>
+      <c r="H21">
+        <v>29676.6</v>
+      </c>
+      <c r="I21">
+        <v>31325</v>
+      </c>
+      <c r="J21">
+        <v>34297.300000000003</v>
+      </c>
+      <c r="K21">
+        <v>32881</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22">
+        <v>134260.20000000001</v>
+      </c>
+      <c r="C22">
+        <v>142815.20000000001</v>
+      </c>
+      <c r="D22">
+        <v>148905.4</v>
+      </c>
+      <c r="E22">
+        <v>171165.5</v>
+      </c>
+      <c r="F22">
+        <v>178022.5</v>
+      </c>
+      <c r="G22">
+        <v>182289.1</v>
+      </c>
+      <c r="H22">
+        <v>190523.4</v>
+      </c>
+      <c r="I22">
+        <v>197527.9</v>
+      </c>
+      <c r="J22">
+        <v>205907.20000000001</v>
+      </c>
+      <c r="K22">
+        <v>198853.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23">
+        <v>20069.3</v>
+      </c>
+      <c r="C23">
+        <v>22061.8</v>
+      </c>
+      <c r="D23">
+        <v>21588.5</v>
+      </c>
+      <c r="E23">
+        <v>22375.4</v>
+      </c>
+      <c r="F23">
+        <v>23179.9</v>
+      </c>
+      <c r="G23">
+        <v>24377.4</v>
+      </c>
+      <c r="H23">
+        <v>24489.8</v>
+      </c>
+      <c r="I23">
+        <v>25383.7</v>
+      </c>
+      <c r="J23">
+        <v>25946</v>
+      </c>
+      <c r="K23">
+        <v>28113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24">
+        <v>15119.7</v>
+      </c>
+      <c r="C24">
+        <v>14954.4</v>
+      </c>
+      <c r="D24">
+        <v>14897.4</v>
+      </c>
+      <c r="E24">
+        <v>14793.7</v>
+      </c>
+      <c r="F24">
+        <v>15925.9</v>
+      </c>
+      <c r="G24">
+        <v>16668.400000000001</v>
+      </c>
+      <c r="H24">
+        <v>16161.7</v>
+      </c>
+      <c r="I24">
+        <v>15889.9</v>
+      </c>
+      <c r="J24">
+        <v>15758</v>
+      </c>
+      <c r="K24">
+        <v>16572.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726719F2-C174-480B-8B54-6F65878C9911}">
+  <dimension ref="C1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="17" customWidth="1"/>
+    <col min="5" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+    </row>
+    <row r="2" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="39">
+        <v>2014</v>
+      </c>
+      <c r="F2" s="39">
+        <v>2015</v>
+      </c>
+      <c r="G2" s="39">
+        <v>2016</v>
+      </c>
+      <c r="H2" s="39">
+        <v>2017</v>
+      </c>
+      <c r="I2" s="39">
+        <v>2018</v>
+      </c>
+      <c r="J2" s="39">
+        <v>2019</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40">
+        <v>6742366</v>
+      </c>
+      <c r="F3" s="40">
+        <v>6917372</v>
+      </c>
+      <c r="G3" s="40">
+        <v>6462938</v>
+      </c>
+      <c r="H3" s="40">
+        <v>6838063</v>
+      </c>
+      <c r="I3" s="40">
+        <v>7444697</v>
+      </c>
+      <c r="J3" s="40">
+        <v>7722799</v>
+      </c>
+      <c r="K3" s="39">
+        <v>6113896</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40">
+        <v>400508</v>
+      </c>
+      <c r="F4" s="40">
+        <v>281579</v>
+      </c>
+      <c r="G4" s="40">
+        <v>464982</v>
+      </c>
+      <c r="H4" s="40">
+        <v>480131</v>
+      </c>
+      <c r="I4" s="40">
+        <v>450576</v>
+      </c>
+      <c r="J4" s="40">
+        <v>479443</v>
+      </c>
+      <c r="K4" s="39">
+        <v>366177</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40">
+        <v>816001</v>
+      </c>
+      <c r="F5" s="40">
+        <v>694570</v>
+      </c>
+      <c r="G5" s="40">
+        <v>755330</v>
+      </c>
+      <c r="H5" s="40">
+        <v>798782</v>
+      </c>
+      <c r="I5" s="40">
+        <v>589341</v>
+      </c>
+      <c r="J5" s="40">
+        <v>698392</v>
+      </c>
+      <c r="K5" s="39">
+        <v>627017</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40">
+        <v>2716098</v>
+      </c>
+      <c r="F6" s="40">
+        <v>3001087</v>
+      </c>
+      <c r="G6" s="40">
+        <v>2764687</v>
+      </c>
+      <c r="H6" s="40">
+        <v>3282957</v>
+      </c>
+      <c r="I6" s="40">
+        <v>3159966</v>
+      </c>
+      <c r="J6" s="40">
+        <v>2923452</v>
+      </c>
+      <c r="K6" s="39">
+        <v>2300526</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40">
+        <v>8326</v>
+      </c>
+      <c r="F7" s="40">
+        <v>7842</v>
+      </c>
+      <c r="G7" s="40">
+        <v>10681</v>
+      </c>
+      <c r="H7" s="40">
+        <v>15184</v>
+      </c>
+      <c r="I7" s="40">
+        <v>16475</v>
+      </c>
+      <c r="J7" s="40">
+        <v>14366</v>
+      </c>
+      <c r="K7" s="39">
+        <v>7578</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40">
+        <v>580120</v>
+      </c>
+      <c r="F8" s="40">
+        <v>748773</v>
+      </c>
+      <c r="G8" s="40">
+        <v>596709</v>
+      </c>
+      <c r="H8" s="40">
+        <v>868871</v>
+      </c>
+      <c r="I8" s="40">
+        <v>835939</v>
+      </c>
+      <c r="J8" s="40">
+        <v>638521</v>
+      </c>
+      <c r="K8" s="39"/>
+    </row>
+    <row r="9" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40">
+        <f>SUM(E3:E8)</f>
+        <v>11263419</v>
+      </c>
+      <c r="F9" s="40">
+        <f t="shared" ref="F9:J9" si="0">SUM(F3:F8)</f>
+        <v>11651223</v>
+      </c>
+      <c r="G9" s="40">
+        <f t="shared" si="0"/>
+        <v>11055327</v>
+      </c>
+      <c r="H9" s="40">
+        <f t="shared" si="0"/>
+        <v>12283988</v>
+      </c>
+      <c r="I9" s="40">
+        <f t="shared" si="0"/>
+        <v>12496994</v>
+      </c>
+      <c r="J9" s="40">
+        <f t="shared" si="0"/>
+        <v>12476973</v>
+      </c>
+      <c r="K9" s="39"/>
+    </row>
+    <row r="10" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="C11" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="F11" s="42">
+        <v>0</v>
+      </c>
+      <c r="G11" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="H11" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="I11" s="43">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="43">
+        <v>7147000</v>
+      </c>
+      <c r="E12" s="43">
+        <v>7147000</v>
+      </c>
+      <c r="F12" s="43">
+        <v>7147000</v>
+      </c>
+      <c r="G12" s="43">
+        <v>7400000</v>
+      </c>
+      <c r="H12" s="43">
+        <v>7400000</v>
+      </c>
+      <c r="I12" s="43">
+        <v>7400000</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="43">
+        <v>6620000</v>
+      </c>
+      <c r="E13" s="43">
+        <v>8160000</v>
+      </c>
+      <c r="F13" s="43">
+        <v>9257000</v>
+      </c>
+      <c r="G13" s="43">
+        <v>8900000</v>
+      </c>
+      <c r="H13" s="43">
+        <v>8900000</v>
+      </c>
+      <c r="I13" s="43">
+        <v>8900000</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="43">
+        <v>570000</v>
+      </c>
+      <c r="E14" s="43">
+        <v>570000</v>
+      </c>
+      <c r="F14" s="43">
+        <v>570000</v>
+      </c>
+      <c r="G14" s="43">
+        <v>400000</v>
+      </c>
+      <c r="H14" s="43">
+        <v>400000</v>
+      </c>
+      <c r="I14" s="43">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42">
+        <v>0</v>
+      </c>
+      <c r="G15" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="H15" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="I15" s="43">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="43">
+        <v>13120000</v>
+      </c>
+      <c r="E16" s="43">
+        <v>13120000</v>
+      </c>
+      <c r="F16" s="43">
+        <v>13120000</v>
+      </c>
+      <c r="G16" s="43">
+        <v>19200000</v>
+      </c>
+      <c r="H16" s="43">
+        <v>19200000</v>
+      </c>
+      <c r="I16" s="43">
+        <v>19200000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="43">
+        <v>5500000</v>
+      </c>
+      <c r="E17" s="43">
+        <v>5500000</v>
+      </c>
+      <c r="F17" s="43">
+        <v>5500000</v>
+      </c>
+      <c r="G17" s="43">
+        <v>7400000</v>
+      </c>
+      <c r="H17" s="43">
+        <v>7400000</v>
+      </c>
+      <c r="I17" s="43">
+        <v>7400000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="43">
+        <v>1500000</v>
+      </c>
+      <c r="E18" s="43">
+        <v>2600000</v>
+      </c>
+      <c r="F18" s="43">
+        <v>2700000</v>
+      </c>
+      <c r="G18" s="43">
+        <v>3850000</v>
+      </c>
+      <c r="H18" s="43">
+        <v>3850000</v>
+      </c>
+      <c r="I18" s="43">
+        <v>3850000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="43">
+        <v>8700000</v>
+      </c>
+      <c r="E19" s="43">
+        <v>10700000</v>
+      </c>
+      <c r="F19" s="43">
+        <v>10700000</v>
+      </c>
+      <c r="G19" s="43">
+        <v>15531000</v>
+      </c>
+      <c r="H19" s="43">
+        <v>15531480</v>
+      </c>
+      <c r="I19" s="43">
+        <v>15531000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="42">
+        <v>0</v>
+      </c>
+      <c r="E20" s="42">
+        <v>0</v>
+      </c>
+      <c r="F20" s="42">
+        <v>0</v>
+      </c>
+      <c r="G20" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="H20" s="43">
+        <v>1800000</v>
+      </c>
+      <c r="I20" s="43">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="43">
+        <v>21100000</v>
+      </c>
+      <c r="E21" s="43">
+        <v>23100000</v>
+      </c>
+      <c r="F21" s="43">
+        <v>23100000</v>
+      </c>
+      <c r="G21" s="43">
+        <v>25500000</v>
+      </c>
+      <c r="H21" s="43">
+        <v>25500000</v>
+      </c>
+      <c r="I21" s="43">
+        <v>25500000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="42">
+        <v>0</v>
+      </c>
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+      <c r="F22" s="42">
+        <v>0</v>
+      </c>
+      <c r="G22" s="43">
+        <v>6700000</v>
+      </c>
+      <c r="H22" s="43">
+        <v>6700000</v>
+      </c>
+      <c r="I22" s="43">
+        <v>8700000</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="42">
+        <v>0</v>
+      </c>
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+      <c r="F23" s="42">
+        <v>0</v>
+      </c>
+      <c r="G23" s="43">
+        <v>7690000</v>
+      </c>
+      <c r="H23" s="43">
+        <v>7690000</v>
+      </c>
+      <c r="I23" s="43">
+        <v>7690000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3117AF2-88D3-406E-BE82-4688F0C37DE5}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5">
+        <v>2010</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2011</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2012</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2013</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="44">
+        <v>2828</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3491</v>
+      </c>
+      <c r="E4" s="44">
+        <v>4035</v>
+      </c>
+      <c r="F4" s="44">
+        <v>4494</v>
+      </c>
+      <c r="G4" s="45">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H4" s="44">
+        <v>6207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="5">
+        <v>712</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1059</v>
+      </c>
+      <c r="E5" s="44">
+        <v>1534</v>
+      </c>
+      <c r="F5" s="44">
+        <v>1701</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="H5" s="44">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="44">
+        <v>1765</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1982</v>
+      </c>
+      <c r="E6" s="44">
+        <v>2136</v>
+      </c>
+      <c r="F6" s="44">
+        <v>2152</v>
+      </c>
+      <c r="G6" s="45">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H6" s="44">
+        <v>2670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="44">
+        <v>1664</v>
+      </c>
+      <c r="D7" s="44">
+        <v>1745</v>
+      </c>
+      <c r="E7" s="44">
+        <v>1979</v>
+      </c>
+      <c r="F7" s="44">
+        <v>2085</v>
+      </c>
+      <c r="G7" s="45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H7" s="44">
+        <v>3364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="5">
+        <v>294</v>
+      </c>
+      <c r="D8" s="5">
+        <v>308</v>
+      </c>
+      <c r="E8" s="5">
+        <v>349</v>
+      </c>
+      <c r="F8" s="5">
+        <v>368</v>
+      </c>
+      <c r="G8" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="H8" s="5">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="5">
+        <v>953</v>
+      </c>
+      <c r="D9" s="44">
+        <v>1041</v>
+      </c>
+      <c r="E9" s="44">
+        <v>1228</v>
+      </c>
+      <c r="F9" s="44">
+        <v>1361</v>
+      </c>
+      <c r="G9" s="45">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H9" s="44">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="47">
+        <f>SUM(C4:C9)</f>
+        <v>8216</v>
+      </c>
+      <c r="D10" s="47">
+        <f t="shared" ref="D10:F10" si="0">SUM(D4:D9)</f>
+        <v>9626</v>
+      </c>
+      <c r="E10" s="47">
+        <f t="shared" si="0"/>
+        <v>11261</v>
+      </c>
+      <c r="F10" s="47">
+        <f t="shared" si="0"/>
+        <v>12161</v>
+      </c>
+      <c r="G10" s="48">
+        <f>AVERAGE(G4:G9)</f>
+        <v>6.0666666666666667E-2</v>
+      </c>
+      <c r="H10" s="47">
+        <f>SUM(H4:H9)</f>
+        <v>17460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3">
+        <v>731</v>
+      </c>
+      <c r="D11" s="3">
+        <v>716</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1050</v>
+      </c>
+      <c r="F11" s="49">
+        <v>1343</v>
+      </c>
+      <c r="G11" s="50">
+        <v>0.15</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="3">
+        <v>519</v>
+      </c>
+      <c r="D12" s="3">
+        <v>581</v>
+      </c>
+      <c r="E12" s="3">
+        <v>676</v>
+      </c>
+      <c r="F12" s="3">
+        <v>771</v>
+      </c>
+      <c r="G12" s="50">
+        <v>0.09</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="3">
+        <v>216</v>
+      </c>
+      <c r="D13" s="3">
+        <v>236</v>
+      </c>
+      <c r="E13" s="3">
+        <v>222</v>
+      </c>
+      <c r="F13" s="3">
+        <v>227</v>
+      </c>
+      <c r="G13" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="H13" s="3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="3">
+        <v>432</v>
+      </c>
+      <c r="D14" s="3">
+        <v>412</v>
+      </c>
+      <c r="E14" s="3">
+        <v>413</v>
+      </c>
+      <c r="F14" s="3">
+        <v>409</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="H14" s="3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="3">
+        <v>200</v>
+      </c>
+      <c r="D15" s="3">
+        <v>202</v>
+      </c>
+      <c r="E15" s="3">
+        <v>204</v>
+      </c>
+      <c r="F15" s="3">
+        <v>206</v>
+      </c>
+      <c r="G15" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="H15" s="3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="3">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3">
+        <v>51</v>
+      </c>
+      <c r="F16" s="3">
+        <v>52</v>
+      </c>
+      <c r="G16" s="50">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>2000</v>
+      </c>
+      <c r="B20" s="17">
+        <f t="shared" ref="B20:B28" si="1">B21/(1+$B$42)</f>
+        <v>4099.3271321821476</v>
+      </c>
+      <c r="C20" s="17">
+        <f>B20*1000000</f>
+        <v>4099327132.1821475</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>2001</v>
+      </c>
+      <c r="B21" s="17">
+        <f t="shared" si="1"/>
+        <v>4394.4786856992623</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>2002</v>
+      </c>
+      <c r="B22" s="17">
+        <f t="shared" si="1"/>
+        <v>4710.8811510696096</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>2003</v>
+      </c>
+      <c r="B23" s="17">
+        <f t="shared" si="1"/>
+        <v>5050.0645939466222</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>2004</v>
+      </c>
+      <c r="B24" s="17">
+        <f t="shared" si="1"/>
+        <v>5413.6692447107789</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>2005</v>
+      </c>
+      <c r="B25" s="17">
+        <f t="shared" si="1"/>
+        <v>5803.4534303299552</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>2006</v>
+      </c>
+      <c r="B26" s="17">
+        <f t="shared" si="1"/>
+        <v>6221.3020773137123</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>2007</v>
+      </c>
+      <c r="B27" s="17">
+        <f t="shared" si="1"/>
+        <v>6669.2358268803</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>2008</v>
+      </c>
+      <c r="B28" s="17">
+        <f t="shared" si="1"/>
+        <v>7149.4208064156819</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>2009</v>
+      </c>
+      <c r="B29" s="17">
+        <f>B30/(1+$B$42)</f>
+        <v>7664.1791044776119</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>2010</v>
+      </c>
+      <c r="B30" s="17">
+        <v>8216</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
+        <v>2011</v>
+      </c>
+      <c r="B31" s="17">
+        <v>9626</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>2012</v>
+      </c>
+      <c r="B32" s="17">
+        <v>11261</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>2013</v>
+      </c>
+      <c r="B33" s="17">
+        <v>12161</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>2014</v>
+      </c>
+      <c r="B34" s="17">
+        <f>B33*(1+$B$41)</f>
+        <v>12723.413960861115</v>
+      </c>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>2015</v>
+      </c>
+      <c r="B35" s="17">
+        <f t="shared" ref="B35:B39" si="2">B34*(1+$B$41)</f>
+        <v>13311.838074125115</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>2016</v>
+      </c>
+      <c r="B36" s="17">
+        <f t="shared" si="2"/>
+        <v>13927.475240280077</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>2017</v>
+      </c>
+      <c r="B37" s="17">
+        <f t="shared" si="2"/>
+        <v>14571.583990767784</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>2018</v>
+      </c>
+      <c r="B38" s="17">
+        <f t="shared" si="2"/>
+        <v>15245.481060767628</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <v>2019</v>
+      </c>
+      <c r="B39" s="17">
+        <f t="shared" si="2"/>
+        <v>15950.544080964934</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>2020</v>
+      </c>
+      <c r="B40" s="17">
+        <v>17460</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="17">
+        <f>(B40/B33)^(1/COUNT(A33:A40))-1</f>
+        <v>4.6247344861533923E-2</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="17">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1707,7 +4133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C97851A-2824-48BF-8D8C-C206FE756299}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1724,18 +4150,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
@@ -1805,7 +4231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D60241-57A3-4230-AFBC-02450A5A3357}">
   <dimension ref="A2:Y24"/>
   <sheetViews>
@@ -1843,31 +4269,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -3120,12 +5546,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB8CE4D-02FD-4279-8CC7-68132636FCCB}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,23 +5563,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="42"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="56"/>
     </row>
     <row r="2" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="17">
@@ -3968,22 +6394,22 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
@@ -4038,7 +6464,7 @@
       <c r="C21" s="21">
         <v>92399</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="57">
         <f>C21+C22</f>
         <v>127577</v>
       </c>
@@ -4086,7 +6512,7 @@
       <c r="C22" s="21">
         <v>35178</v>
       </c>
-      <c r="D22" s="43"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="21">
         <v>61307</v>
       </c>
@@ -4131,7 +6557,7 @@
       <c r="C23" s="21">
         <v>67598</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="62">
         <f>SUM(C23:C25)</f>
         <v>106762</v>
       </c>
@@ -4179,7 +6605,7 @@
       <c r="C24" s="21">
         <v>24073</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="63"/>
       <c r="E24" s="21">
         <v>27771</v>
       </c>
@@ -4224,7 +6650,7 @@
       <c r="C25" s="21">
         <v>15091</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="63"/>
       <c r="E25" s="21">
         <v>17657</v>
       </c>
@@ -4317,7 +6743,7 @@
       <c r="C27" s="21">
         <v>37027</v>
       </c>
-      <c r="D27" s="50">
+      <c r="D27" s="64">
         <f>SUM(C27:C28)</f>
         <v>48633</v>
       </c>
@@ -4365,7 +6791,7 @@
       <c r="C28" s="21">
         <v>11606</v>
       </c>
-      <c r="D28" s="51"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="21">
         <v>3757</v>
       </c>
@@ -4455,7 +6881,7 @@
       <c r="C30" s="9">
         <v>61388</v>
       </c>
-      <c r="D30" s="43">
+      <c r="D30" s="57">
         <f>C30+C31</f>
         <v>95893</v>
       </c>
@@ -4503,7 +6929,7 @@
       <c r="C31" s="9">
         <v>34505</v>
       </c>
-      <c r="D31" s="44"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="21">
         <v>33435</v>
       </c>
@@ -4638,7 +7064,7 @@
       <c r="C34" s="9">
         <v>18663</v>
       </c>
-      <c r="D34" s="43">
+      <c r="D34" s="57">
         <f>C34+C35</f>
         <v>24401</v>
       </c>
@@ -4686,7 +7112,7 @@
       <c r="C35" s="9">
         <v>5738</v>
       </c>
-      <c r="D35" s="44"/>
+      <c r="D35" s="58"/>
       <c r="E35" s="21">
         <v>37324</v>
       </c>
@@ -5080,40 +7506,40 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="47"/>
-      <c r="M44" s="47"/>
-      <c r="N44" s="47"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="M45" s="47"/>
-      <c r="N45" s="47"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D46" s="25">
@@ -5137,12 +7563,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDB59F0-D6B3-4A6B-A133-7B17C332CA6B}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5270,11 +7696,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0A275E-95A3-45C9-8796-8D4F4C7E0B61}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81DEF2E-0707-41F9-9B0C-871BA79BADE8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>